<commit_message>
finished the 1st circuit and started slides
</commit_message>
<xml_diff>
--- a/project/fault_analysis_1.xlsx
+++ b/project/fault_analysis_1.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Fault Analysis" sheetId="1" r:id="rId1"/>
+    <sheet name="FA TT" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="41">
   <si>
     <t>A</t>
   </si>
@@ -103,12 +104,57 @@
   <si>
     <t xml:space="preserve">Testability </t>
   </si>
+  <si>
+    <t>Input</t>
+  </si>
+  <si>
+    <t>Output</t>
+  </si>
+  <si>
+    <t>Sum</t>
+  </si>
+  <si>
+    <t>Carry</t>
+  </si>
+  <si>
+    <t>HD = 68.75%</t>
+  </si>
+  <si>
+    <t>Encrypt Output W/ Key 1</t>
+  </si>
+  <si>
+    <t>Encrypt Output W/ Key 2</t>
+  </si>
+  <si>
+    <t>HD = 62.5%</t>
+  </si>
+  <si>
+    <t>Encrypt Output W/ Key 3</t>
+  </si>
+  <si>
+    <t>HD = 50%</t>
+  </si>
+  <si>
+    <t>SW13</t>
+  </si>
+  <si>
+    <t>SW14</t>
+  </si>
+  <si>
+    <t>SW15</t>
+  </si>
+  <si>
+    <t>Encryption Key</t>
+  </si>
+  <si>
+    <t>when SW13 = 0, SW14 = 1, SW15 = 0</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -129,16 +175,43 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="14">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -321,11 +394,63 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -379,6 +504,45 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -697,8 +861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BD32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1102,10 +1266,10 @@
       </c>
     </row>
     <row r="4" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+      <c r="A4" s="30">
         <v>8</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="30">
         <v>0.375</v>
       </c>
       <c r="D4" s="1">
@@ -1214,10 +1378,10 @@
       </c>
     </row>
     <row r="5" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+      <c r="A5" s="30">
         <v>15</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="30">
         <v>0.375</v>
       </c>
       <c r="D5" s="1">
@@ -1458,10 +1622,10 @@
       </c>
     </row>
     <row r="7" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+      <c r="A7" s="30">
         <v>11</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="30">
         <v>0.25</v>
       </c>
       <c r="D7" s="1">
@@ -3844,11 +4008,6 @@
     <sortCondition descending="1" ref="B2:B17"/>
   </sortState>
   <mergeCells count="12">
-    <mergeCell ref="AE10:AG10"/>
-    <mergeCell ref="AE32:AG32"/>
-    <mergeCell ref="AN10:AP10"/>
-    <mergeCell ref="AN32:AP32"/>
-    <mergeCell ref="AW10:AY10"/>
     <mergeCell ref="D10:F10"/>
     <mergeCell ref="D21:F21"/>
     <mergeCell ref="D32:F32"/>
@@ -3856,8 +4015,439 @@
     <mergeCell ref="V10:X10"/>
     <mergeCell ref="M32:O32"/>
     <mergeCell ref="V21:X21"/>
+    <mergeCell ref="AE10:AG10"/>
+    <mergeCell ref="AE32:AG32"/>
+    <mergeCell ref="AN10:AP10"/>
+    <mergeCell ref="AN32:AP32"/>
+    <mergeCell ref="AW10:AY10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M27" sqref="M27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="3" width="6.140625" style="24" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.140625" style="24" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.5703125" style="24" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="24"/>
+    <col min="7" max="7" width="16.85546875" style="24" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="24"/>
+    <col min="9" max="9" width="16.7109375" style="24" customWidth="1"/>
+    <col min="10" max="11" width="20.7109375" style="24" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="24"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="20"/>
+      <c r="F1" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="K1" s="28"/>
+    </row>
+    <row r="2" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="J2" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="K2" s="22" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0</v>
+      </c>
+      <c r="C3" s="23">
+        <v>0</v>
+      </c>
+      <c r="D3" s="26">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0</v>
+      </c>
+      <c r="F3" s="26">
+        <v>1</v>
+      </c>
+      <c r="G3" s="2">
+        <v>0</v>
+      </c>
+      <c r="H3" s="26">
+        <v>1</v>
+      </c>
+      <c r="I3" s="2">
+        <v>0</v>
+      </c>
+      <c r="J3" s="26">
+        <v>1</v>
+      </c>
+      <c r="K3" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>0</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0</v>
+      </c>
+      <c r="C4" s="9">
+        <v>1</v>
+      </c>
+      <c r="D4" s="12">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0</v>
+      </c>
+      <c r="F4" s="12">
+        <v>0</v>
+      </c>
+      <c r="G4" s="1">
+        <v>1</v>
+      </c>
+      <c r="H4" s="12">
+        <v>0</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0</v>
+      </c>
+      <c r="J4" s="12">
+        <v>0</v>
+      </c>
+      <c r="K4" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>0</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="9">
+        <v>0</v>
+      </c>
+      <c r="D5" s="12">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0</v>
+      </c>
+      <c r="F5" s="12">
+        <v>0</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0</v>
+      </c>
+      <c r="H5" s="12">
+        <v>0</v>
+      </c>
+      <c r="I5" s="1">
+        <v>0</v>
+      </c>
+      <c r="J5" s="12">
+        <v>0</v>
+      </c>
+      <c r="K5" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>0</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+      <c r="C6" s="9">
+        <v>1</v>
+      </c>
+      <c r="D6" s="12">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>1</v>
+      </c>
+      <c r="F6" s="12">
+        <v>1</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0</v>
+      </c>
+      <c r="H6" s="12">
+        <v>1</v>
+      </c>
+      <c r="I6" s="1">
+        <v>0</v>
+      </c>
+      <c r="J6" s="12">
+        <v>1</v>
+      </c>
+      <c r="K6" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>1</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0</v>
+      </c>
+      <c r="C7" s="9">
+        <v>0</v>
+      </c>
+      <c r="D7" s="12">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0</v>
+      </c>
+      <c r="F7" s="12">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0</v>
+      </c>
+      <c r="H7" s="12">
+        <v>0</v>
+      </c>
+      <c r="I7" s="1">
+        <v>0</v>
+      </c>
+      <c r="J7" s="12">
+        <v>0</v>
+      </c>
+      <c r="K7" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>1</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0</v>
+      </c>
+      <c r="C8" s="9">
+        <v>1</v>
+      </c>
+      <c r="D8" s="12">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1">
+        <v>1</v>
+      </c>
+      <c r="F8" s="12">
+        <v>1</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0</v>
+      </c>
+      <c r="H8" s="12">
+        <v>1</v>
+      </c>
+      <c r="I8" s="1">
+        <v>0</v>
+      </c>
+      <c r="J8" s="12">
+        <v>1</v>
+      </c>
+      <c r="K8" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>1</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1</v>
+      </c>
+      <c r="C9" s="9">
+        <v>0</v>
+      </c>
+      <c r="D9" s="12">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1">
+        <v>1</v>
+      </c>
+      <c r="F9" s="12">
+        <v>1</v>
+      </c>
+      <c r="G9" s="1">
+        <v>1</v>
+      </c>
+      <c r="H9" s="12">
+        <v>1</v>
+      </c>
+      <c r="I9" s="1">
+        <v>1</v>
+      </c>
+      <c r="J9" s="12">
+        <v>1</v>
+      </c>
+      <c r="K9" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>1</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1</v>
+      </c>
+      <c r="C10" s="9">
+        <v>1</v>
+      </c>
+      <c r="D10" s="12">
+        <v>1</v>
+      </c>
+      <c r="E10" s="1">
+        <v>1</v>
+      </c>
+      <c r="F10" s="12">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1">
+        <v>1</v>
+      </c>
+      <c r="H10" s="12">
+        <v>0</v>
+      </c>
+      <c r="I10" s="1">
+        <v>1</v>
+      </c>
+      <c r="J10" s="12">
+        <v>0</v>
+      </c>
+      <c r="K10" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F11" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="G11" s="29"/>
+      <c r="H11" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="I11" s="29"/>
+      <c r="J11" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="K11" s="29"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J12" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="K12" s="27"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="31"/>
+      <c r="C14" s="31"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="25" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="25">
+        <v>0</v>
+      </c>
+      <c r="B16" s="25">
+        <v>1</v>
+      </c>
+      <c r="C16" s="25">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="H11:I11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
made corrections to node 8
</commit_message>
<xml_diff>
--- a/project/fault_analysis_1.xlsx
+++ b/project/fault_analysis_1.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="41">
   <si>
     <t>A</t>
   </si>
@@ -856,7 +856,7 @@
   <dimension ref="A1:BD32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2103,7 +2103,7 @@
         <v>8</v>
       </c>
       <c r="B12" s="1">
-        <v>0</v>
+        <v>0.1875</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>0</v>
@@ -2372,11 +2372,21 @@
       <c r="X14" s="9">
         <v>1</v>
       </c>
-      <c r="Y14" s="6"/>
-      <c r="Z14" s="9"/>
-      <c r="AA14" s="12"/>
-      <c r="AB14" s="1"/>
-      <c r="AC14" s="14"/>
+      <c r="Y14" s="6">
+        <v>1</v>
+      </c>
+      <c r="Z14" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA14" s="12">
+        <v>0</v>
+      </c>
+      <c r="AB14" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC14" s="14" t="s">
+        <v>23</v>
+      </c>
       <c r="AE14" s="1">
         <v>0</v>
       </c>
@@ -2582,11 +2592,21 @@
       <c r="X16" s="9">
         <v>1</v>
       </c>
-      <c r="Y16" s="6"/>
-      <c r="Z16" s="9"/>
-      <c r="AA16" s="12"/>
-      <c r="AB16" s="1"/>
-      <c r="AC16" s="14"/>
+      <c r="Y16" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z16" s="9">
+        <v>1</v>
+      </c>
+      <c r="AA16" s="12">
+        <v>1</v>
+      </c>
+      <c r="AB16" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC16" s="14" t="s">
+        <v>22</v>
+      </c>
       <c r="AE16" s="1">
         <v>0</v>
       </c>
@@ -2786,11 +2806,21 @@
       <c r="X18" s="9">
         <v>1</v>
       </c>
-      <c r="Y18" s="6"/>
-      <c r="Z18" s="9"/>
-      <c r="AA18" s="12"/>
-      <c r="AB18" s="1"/>
-      <c r="AC18" s="14"/>
+      <c r="Y18" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z18" s="9">
+        <v>1</v>
+      </c>
+      <c r="AA18" s="12">
+        <v>1</v>
+      </c>
+      <c r="AB18" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC18" s="14" t="s">
+        <v>22</v>
+      </c>
       <c r="AE18" s="1">
         <v>1</v>
       </c>
@@ -3064,7 +3094,7 @@
       <c r="W21" s="24"/>
       <c r="X21" s="24"/>
       <c r="AC21" s="17">
-        <v>0</v>
+        <v>0.1875</v>
       </c>
       <c r="AL21" s="17">
         <v>0.5</v>

</xml_diff>

<commit_message>
Completed the first FA. going to simulate using vivado
</commit_message>
<xml_diff>
--- a/project/fault_analysis_1.xlsx
+++ b/project/fault_analysis_1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Fault Analysis" sheetId="1" r:id="rId1"/>
@@ -117,9 +117,6 @@
     <t>Carry</t>
   </si>
   <si>
-    <t>HD = 68.75%</t>
-  </si>
-  <si>
     <t>Encrypt Output W/ Key 1</t>
   </si>
   <si>
@@ -148,6 +145,9 @@
   </si>
   <si>
     <t>when SW13 = 0, SW14 = 1, SW15 = 0</t>
+  </si>
+  <si>
+    <t>HD = 25%</t>
   </si>
 </sst>
 </file>
@@ -515,6 +515,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -534,9 +537,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -855,8 +855,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BD32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1270,10 +1270,10 @@
       </c>
     </row>
     <row r="4" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A4" s="31">
+      <c r="A4" s="24">
         <v>10</v>
       </c>
-      <c r="B4" s="31">
+      <c r="B4" s="24">
         <v>0.5</v>
       </c>
       <c r="D4" s="1">
@@ -1392,10 +1392,10 @@
       </c>
     </row>
     <row r="5" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A5" s="31">
+      <c r="A5" s="24">
         <v>11</v>
       </c>
-      <c r="B5" s="31">
+      <c r="B5" s="24">
         <v>0.5</v>
       </c>
       <c r="D5" s="1">
@@ -1514,10 +1514,10 @@
       </c>
     </row>
     <row r="6" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A6" s="31">
+      <c r="A6" s="24">
         <v>9</v>
       </c>
-      <c r="B6" s="31">
+      <c r="B6" s="24">
         <v>0.375</v>
       </c>
       <c r="D6" s="1">
@@ -1646,10 +1646,10 @@
       </c>
     </row>
     <row r="7" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A7" s="31">
+      <c r="A7" s="24">
         <v>15</v>
       </c>
-      <c r="B7" s="31">
+      <c r="B7" s="24">
         <v>0.375</v>
       </c>
       <c r="D7" s="1">
@@ -2018,11 +2018,11 @@
       <c r="B10" s="1">
         <v>0.1875</v>
       </c>
-      <c r="D10" s="24" t="s">
+      <c r="D10" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="24"/>
-      <c r="F10" s="24"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
       <c r="G10" s="14"/>
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
@@ -2041,11 +2041,11 @@
         <v>0</v>
       </c>
       <c r="U10" s="17"/>
-      <c r="V10" s="24" t="s">
+      <c r="V10" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="W10" s="24"/>
-      <c r="X10" s="24"/>
+      <c r="W10" s="25"/>
+      <c r="X10" s="25"/>
       <c r="Y10" s="14"/>
       <c r="Z10" s="14"/>
       <c r="AA10" s="14"/>
@@ -2053,11 +2053,11 @@
       <c r="AC10" s="13">
         <v>0.1875</v>
       </c>
-      <c r="AE10" s="24" t="s">
+      <c r="AE10" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="AF10" s="24"/>
-      <c r="AG10" s="24"/>
+      <c r="AF10" s="25"/>
+      <c r="AG10" s="25"/>
       <c r="AH10" s="14"/>
       <c r="AI10" s="14"/>
       <c r="AJ10" s="14"/>
@@ -2065,11 +2065,11 @@
       <c r="AL10" s="13">
         <v>0.5</v>
       </c>
-      <c r="AN10" s="24" t="s">
+      <c r="AN10" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="AO10" s="24"/>
-      <c r="AP10" s="24"/>
+      <c r="AO10" s="25"/>
+      <c r="AP10" s="25"/>
       <c r="AQ10" s="14"/>
       <c r="AR10" s="14"/>
       <c r="AS10" s="14"/>
@@ -2077,11 +2077,11 @@
       <c r="AU10" s="13">
         <v>0.25</v>
       </c>
-      <c r="AW10" s="24" t="s">
+      <c r="AW10" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="AX10" s="24"/>
-      <c r="AY10" s="24"/>
+      <c r="AX10" s="25"/>
+      <c r="AY10" s="25"/>
       <c r="AZ10" s="14"/>
       <c r="BA10" s="14"/>
       <c r="BB10" s="14"/>
@@ -3076,11 +3076,11 @@
       <c r="BC20" s="14"/>
     </row>
     <row r="21" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="D21" s="24" t="s">
+      <c r="D21" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="E21" s="24"/>
-      <c r="F21" s="24"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="25"/>
       <c r="K21" s="17">
         <v>0</v>
       </c>
@@ -3088,11 +3088,11 @@
         <v>0</v>
       </c>
       <c r="U21" s="17"/>
-      <c r="V21" s="24" t="s">
+      <c r="V21" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="W21" s="24"/>
-      <c r="X21" s="24"/>
+      <c r="W21" s="25"/>
+      <c r="X21" s="25"/>
       <c r="AC21" s="17">
         <v>0.1875</v>
       </c>
@@ -4055,44 +4055,44 @@
       <c r="BC31" s="14"/>
     </row>
     <row r="32" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="D32" s="24" t="s">
+      <c r="D32" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="E32" s="24"/>
-      <c r="F32" s="24"/>
+      <c r="E32" s="25"/>
+      <c r="F32" s="25"/>
       <c r="K32" s="17">
         <v>0</v>
       </c>
-      <c r="M32" s="24" t="s">
+      <c r="M32" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="N32" s="24"/>
-      <c r="O32" s="24"/>
+      <c r="N32" s="25"/>
+      <c r="O32" s="25"/>
       <c r="T32" s="17">
         <v>0.1875</v>
       </c>
       <c r="U32" s="17"/>
-      <c r="V32" s="24" t="s">
+      <c r="V32" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="W32" s="24"/>
-      <c r="X32" s="24"/>
+      <c r="W32" s="25"/>
+      <c r="X32" s="25"/>
       <c r="AC32" s="17">
         <v>0.375</v>
       </c>
-      <c r="AE32" s="24" t="s">
+      <c r="AE32" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="AF32" s="24"/>
-      <c r="AG32" s="24"/>
+      <c r="AF32" s="25"/>
+      <c r="AG32" s="25"/>
       <c r="AL32" s="17">
         <v>0.1875</v>
       </c>
-      <c r="AN32" s="24" t="s">
+      <c r="AN32" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="AO32" s="24"/>
-      <c r="AP32" s="24"/>
+      <c r="AO32" s="25"/>
+      <c r="AP32" s="25"/>
       <c r="AU32" s="17">
         <v>0.375</v>
       </c>
@@ -4102,6 +4102,11 @@
     <sortCondition descending="1" ref="B2:B17"/>
   </sortState>
   <mergeCells count="12">
+    <mergeCell ref="AE10:AG10"/>
+    <mergeCell ref="AE32:AG32"/>
+    <mergeCell ref="AN10:AP10"/>
+    <mergeCell ref="AN32:AP32"/>
+    <mergeCell ref="AW10:AY10"/>
     <mergeCell ref="D10:F10"/>
     <mergeCell ref="D21:F21"/>
     <mergeCell ref="D32:F32"/>
@@ -4109,11 +4114,6 @@
     <mergeCell ref="V10:X10"/>
     <mergeCell ref="M32:O32"/>
     <mergeCell ref="V21:X21"/>
-    <mergeCell ref="AE10:AG10"/>
-    <mergeCell ref="AE32:AG32"/>
-    <mergeCell ref="AN10:AP10"/>
-    <mergeCell ref="AN32:AP32"/>
-    <mergeCell ref="AW10:AY10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967295" r:id="rId1"/>
@@ -4124,8 +4124,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M27" sqref="M27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4142,27 +4142,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="30" t="s">
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="30"/>
-      <c r="F1" s="25" t="s">
+      <c r="E1" s="31"/>
+      <c r="F1" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25" t="s">
-        <v>32</v>
-      </c>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="K1" s="25"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="K1" s="26"/>
     </row>
     <row r="2" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -4254,7 +4254,7 @@
         <v>0</v>
       </c>
       <c r="G4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H4" s="12">
         <v>0</v>
@@ -4324,7 +4324,7 @@
         <v>1</v>
       </c>
       <c r="G6" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6" s="12">
         <v>1</v>
@@ -4394,7 +4394,7 @@
         <v>1</v>
       </c>
       <c r="G8" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8" s="12">
         <v>1</v>
@@ -4480,41 +4480,41 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F11" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="G11" s="26"/>
-      <c r="H11" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="I11" s="26"/>
-      <c r="J11" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="K11" s="26"/>
+      <c r="F11" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="G11" s="27"/>
+      <c r="H11" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="I11" s="27"/>
+      <c r="J11" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="K11" s="27"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="J12" s="28" t="s">
-        <v>40</v>
-      </c>
-      <c r="K12" s="28"/>
+      <c r="J12" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="K12" s="29"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="27" t="s">
-        <v>39</v>
-      </c>
-      <c r="B14" s="27"/>
-      <c r="C14" s="27"/>
+      <c r="A14" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="28"/>
+      <c r="C14" s="28"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="B15" s="22" t="s">
+      <c r="C15" s="22" t="s">
         <v>37</v>
-      </c>
-      <c r="C15" s="22" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>